<commit_message>
Criada a classe gráfico
</commit_message>
<xml_diff>
--- a/homicidiosHomensNaoNegrosPais.xlsx
+++ b/homicidiosHomensNaoNegrosPais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zsg-k\IdeaProjects\guiExample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95EBCEF-0549-43C2-9604-7DF0E89456B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B93C883-45BD-4874-A0C8-69BF63A47CC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -629,6 +629,76 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="7" formatCode="#,##0.00_);\(#,##0.00\)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="7" formatCode="#,##0.00_);\(#,##0.00\)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -810,41 +880,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="3"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="7" formatCode="#,##0.00_);\(#,##0.00\)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -858,41 +893,6 @@
         <right/>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="3"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="7" formatCode="#,##0.00_);\(#,##0.00\)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1175,13 +1175,13 @@
     <tableColumn id="8" xr3:uid="{49D7879F-3962-4B85-A110-BFF0CBFCA36D}" name="Coluna1" headerRowDxfId="15" dataDxfId="14" dataCellStyle="Título 3"/>
     <tableColumn id="9" xr3:uid="{DCC3A56A-463F-4799-8ED0-BD149DCB1A92}" name="Coluna2" headerRowDxfId="13" dataDxfId="12" dataCellStyle="Título 3"/>
     <tableColumn id="10" xr3:uid="{89AE2600-564D-4AFF-9A88-0358B1225E5B}" name="Coluna3" headerRowDxfId="11" dataDxfId="10" dataCellStyle="Título 3"/>
-    <tableColumn id="4" xr3:uid="{AEC171E9-4165-4FAB-8567-155A4F05EAD9}" name="Coluna4" totalsRowFunction="sum" headerRowDxfId="9" dataDxfId="8" dataCellStyle="Título 3">
+    <tableColumn id="4" xr3:uid="{AEC171E9-4165-4FAB-8567-155A4F05EAD9}" name="Coluna4" totalsRowFunction="sum" headerRowDxfId="9" dataDxfId="0" dataCellStyle="Título 3">
       <calculatedColumnFormula array="1">Desv</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A575222F-848A-48FC-BB7F-6833C1291522}" name="Coluna5" headerRowDxfId="7" dataDxfId="6" headerRowCellStyle="Título 3" dataCellStyle="Título 3"/>
-    <tableColumn id="6" xr3:uid="{8234CFF4-4512-4623-AE93-7A772C47DEF7}" name="Coluna6" headerRowDxfId="5" dataDxfId="4" dataCellStyle="Título 3"/>
-    <tableColumn id="7" xr3:uid="{8935A9A1-0301-4C62-BBB0-D82B52192D37}" name="Coluna7" headerRowDxfId="3" dataDxfId="2" dataCellStyle="Título 3"/>
-    <tableColumn id="11" xr3:uid="{C2612062-0DB6-4768-A486-D120442E70E1}" name="Coluna8" headerRowDxfId="1" dataDxfId="0" dataCellStyle="Título 3"/>
+    <tableColumn id="5" xr3:uid="{A575222F-848A-48FC-BB7F-6833C1291522}" name="Coluna5" headerRowDxfId="8" dataDxfId="1" headerRowCellStyle="Título 3" dataCellStyle="Título 3"/>
+    <tableColumn id="6" xr3:uid="{8234CFF4-4512-4623-AE93-7A772C47DEF7}" name="Coluna6" headerRowDxfId="7" dataDxfId="6" dataCellStyle="Título 3"/>
+    <tableColumn id="7" xr3:uid="{8935A9A1-0301-4C62-BBB0-D82B52192D37}" name="Coluna7" headerRowDxfId="5" dataDxfId="4" dataCellStyle="Título 3"/>
+    <tableColumn id="11" xr3:uid="{C2612062-0DB6-4768-A486-D120442E70E1}" name="Coluna8" headerRowDxfId="3" dataDxfId="2" dataCellStyle="Título 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1487,7 +1487,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,20 +1753,19 @@
         <v>14333.722222222223</v>
       </c>
       <c r="D18" s="11">
-        <f>AVEDEV(B1:B18)</f>
-        <v>1434.5493827160494</v>
+        <f>MEDIAN(B1:B18)</f>
+        <v>13482.5</v>
       </c>
       <c r="E18" s="11">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11">
         <f>_xlfn.STDEV.P(B1:B18)</f>
         <v>1668.4661221065544</v>
       </c>
-      <c r="F18" s="11">
+      <c r="G18" s="11">
         <f>_xlfn.VAR.P(B1:B18)</f>
         <v>2783779.200617284</v>
-      </c>
-      <c r="G18" s="11">
-        <f>E18/C18</f>
-        <v>0.11640145499121334</v>
       </c>
       <c r="H18" s="11">
         <f>_xlfn.VAR.S(B1:B18)</f>

</xml_diff>